<commit_message>
Todos los cambios de la clasificación de datos structurados. Tener en cuenta que para los casos de las tablas de web de tenerife, no se ha generalizado, sólo se ha modificado el index_istac para que extraiga de estas
</commit_message>
<xml_diff>
--- a/airflow/data_analysis/classify_elastic/structured_data/excels_recursos_naturales/recursos.xlsx
+++ b/airflow/data_analysis/classify_elastic/structured_data/excels_recursos_naturales/recursos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempo atmosférico" sheetId="1" state="visible" r:id="rId2"/>
@@ -582,22 +582,22 @@
     <t xml:space="preserve">01/02/2018 - 30/11/2018</t>
   </si>
   <si>
+    <t xml:space="preserve">Sí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apta para el baño</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excelente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playa San Telmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playa Martiánez</t>
+  </si>
+  <si>
     <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apta para el baño</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excelente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Playa San Telmo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Playa Martiánez</t>
   </si>
   <si>
     <t xml:space="preserve">http://www3.gobiernodecanarias.org/sanidad/scs/mapa.jsp?idDocument=e200513a-a2fa-11e0-9610-f1717f4d08a3&amp;idCarpeta=df4c5b0a-acc9-11dd-bcc2-dd39af5a7493</t>
@@ -1087,12 +1087,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4210526315789"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.1052631578947"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="14" min="7" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -3845,16 +3845,16 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -3902,7 +3902,7 @@
         <v>184</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>186</v>
@@ -3913,13 +3913,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>184</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>186</v>
@@ -3960,8 +3960,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -4064,11 +4064,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9554655870445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.5991902834008"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -4110,7 +4110,7 @@
         <v>209</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>210</v>
@@ -4127,7 +4127,7 @@
         <v>213</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>214</v>
@@ -4144,7 +4144,7 @@
         <v>216</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>210</v>
@@ -4161,7 +4161,7 @@
         <v>218</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>214</v>
@@ -4175,7 +4175,7 @@
         <v>220</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>214</v>
@@ -4192,7 +4192,7 @@
         <v>223</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>210</v>
@@ -4209,7 +4209,7 @@
         <v>225</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>226</v>
@@ -4226,7 +4226,7 @@
         <v>229</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>230</v>
@@ -4243,7 +4243,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>230</v>
@@ -4260,7 +4260,7 @@
         <v>234</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>235</v>
@@ -4277,7 +4277,7 @@
         <v>237</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>210</v>
@@ -4294,7 +4294,7 @@
         <v>239</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>240</v>
@@ -4311,7 +4311,7 @@
         <v>243</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>244</v>
@@ -4328,7 +4328,7 @@
         <v>246</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>214</v>
@@ -4345,7 +4345,7 @@
         <v>248</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>214</v>
@@ -4359,7 +4359,7 @@
         <v>250</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>210</v>
@@ -4376,7 +4376,7 @@
         <v>252</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>210</v>
@@ -4393,7 +4393,7 @@
         <v>255</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>210</v>

</xml_diff>